<commit_message>
DXF files prepared for Fabrinox quote
</commit_message>
<xml_diff>
--- a/Hardware/PCB/KiCad_Files/Manufacturing/Hydrogel-Bioprinter-CPL.xlsx
+++ b/Hardware/PCB/KiCad_Files/Manufacturing/Hydrogel-Bioprinter-CPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Projects\Hydrogel-3D-Printer\Hardware\PCB\KiCad_Files\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0D56C16C-AE23-4BEA-ACD4-16E52BF03DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330265AA-7BC2-4C32-B098-7F726B54DEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2359A6F5-FF09-4ADF-86CD-F3C999B48094}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2359A6F5-FF09-4ADF-86CD-F3C999B48094}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrogel-Bioprinter-CPL" sheetId="1" r:id="rId1"/>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E22762-10C9-44B3-9498-A9908225A849}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>